<commit_message>
added work along files for excel module
</commit_message>
<xml_diff>
--- a/Module-7-PB/employee-data.xlsx
+++ b/Module-7-PB/employee-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\research\master-classes\data-analyst-masterclass\Module-7-PB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97262870-B008-4951-A90F-446669C85F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECCC7C8-CC67-4230-8088-03DEA4FAEA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5011D342-9B25-46AA-9B68-1A5D64F959B1}"/>
   </bookViews>
@@ -2148,7 +2148,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3298,7 +3298,7 @@
   <dimension ref="A1:E1097"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26515,7 +26515,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26523,6 +26523,7 @@
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.109375"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>